<commit_message>
added web driver wait protocol
</commit_message>
<xml_diff>
--- a/zipcodes/CanadianPostalCodes202403_Processed.xlsx
+++ b/zipcodes/CanadianPostalCodes202403_Processed.xlsx
@@ -461,7 +461,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -474,7 +478,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -487,7 +495,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -500,7 +512,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -513,7 +529,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -526,7 +546,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -539,7 +563,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -552,7 +580,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -565,7 +597,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -578,7 +614,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -591,7 +631,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -604,7 +648,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -617,7 +665,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -630,7 +682,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -643,7 +699,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -656,7 +716,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -669,7 +733,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -682,7 +750,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -695,7 +767,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -708,7 +784,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -721,7 +801,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -734,7 +818,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -747,7 +835,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -760,7 +852,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -773,7 +869,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -786,7 +886,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -799,7 +903,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -812,7 +920,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -825,7 +937,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -838,7 +954,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -851,7 +971,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -864,7 +988,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -877,7 +1005,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -890,7 +1022,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -903,7 +1039,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -916,7 +1056,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -929,7 +1073,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -942,7 +1090,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -955,7 +1107,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -968,7 +1124,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -981,7 +1141,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -994,7 +1158,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1007,7 +1175,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1020,7 +1192,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1033,7 +1209,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1046,7 +1226,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1059,7 +1243,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1072,7 +1260,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1085,7 +1277,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1098,7 +1294,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1111,7 +1311,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1124,7 +1328,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1137,7 +1345,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1150,7 +1362,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1163,7 +1379,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1176,7 +1396,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1189,7 +1413,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1202,7 +1430,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1215,7 +1447,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1228,7 +1464,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1241,7 +1481,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1254,7 +1498,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1267,7 +1515,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1280,7 +1532,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1293,7 +1549,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1306,7 +1566,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1319,7 +1583,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1332,7 +1600,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1345,7 +1617,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1358,7 +1634,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1371,7 +1651,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1384,7 +1668,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1397,7 +1685,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1410,7 +1702,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1423,7 +1719,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1436,7 +1736,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1449,7 +1753,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1462,7 +1770,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr"/>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1475,7 +1787,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr"/>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1488,7 +1804,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr"/>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1501,7 +1821,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr"/>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1514,7 +1838,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr"/>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1527,7 +1855,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1540,7 +1872,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1553,7 +1889,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1566,7 +1906,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr"/>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1579,7 +1923,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr"/>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1592,7 +1940,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr"/>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1605,7 +1957,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1618,7 +1974,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr"/>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1631,7 +1991,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1644,7 +2008,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr"/>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1657,7 +2025,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr"/>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1670,7 +2042,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr"/>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1683,7 +2059,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr"/>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1696,7 +2076,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr"/>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1709,7 +2093,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr"/>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1722,7 +2110,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr"/>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1735,7 +2127,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr"/>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1748,7 +2144,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr"/>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1761,7 +2161,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr"/>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1774,7 +2178,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr"/>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1787,7 +2195,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr"/>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1800,7 +2212,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr"/>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1813,7 +2229,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr"/>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1826,7 +2246,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr"/>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1839,7 +2263,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr"/>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1852,7 +2280,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr"/>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1865,7 +2297,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr"/>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1878,7 +2314,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr"/>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1891,7 +2331,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr"/>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1904,7 +2348,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr"/>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1917,7 +2365,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr"/>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1930,7 +2382,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr"/>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1943,7 +2399,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1956,7 +2416,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr"/>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1969,7 +2433,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr"/>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1982,7 +2450,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr"/>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -1995,7 +2467,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr"/>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2008,7 +2484,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2021,7 +2501,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr"/>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2034,7 +2518,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr"/>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2047,7 +2535,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr"/>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2060,7 +2552,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr"/>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2073,7 +2569,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr"/>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2086,7 +2586,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr"/>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2099,7 +2603,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr"/>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2112,7 +2620,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr"/>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2125,7 +2637,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr"/>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2138,7 +2654,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr"/>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2151,7 +2671,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C132" t="inlineStr"/>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2164,7 +2688,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C133" t="inlineStr"/>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2177,7 +2705,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr"/>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2190,7 +2722,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr"/>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2203,7 +2739,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C136" t="inlineStr"/>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2216,7 +2756,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr"/>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2229,7 +2773,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr"/>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2242,7 +2790,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr"/>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2255,7 +2807,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr"/>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2268,7 +2824,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr"/>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2281,7 +2841,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C142" t="inlineStr"/>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2294,7 +2858,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C143" t="inlineStr"/>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2307,7 +2875,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C144" t="inlineStr"/>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2320,7 +2892,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C145" t="inlineStr"/>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2333,7 +2909,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C146" t="inlineStr"/>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2346,7 +2926,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C147" t="inlineStr"/>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2359,7 +2943,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C148" t="inlineStr"/>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2372,7 +2960,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C149" t="inlineStr"/>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2385,7 +2977,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C150" t="inlineStr"/>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2398,7 +2994,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C151" t="inlineStr"/>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -2411,7 +3011,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C152" t="inlineStr"/>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -2424,7 +3028,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr"/>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -2437,7 +3045,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr"/>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -2450,7 +3062,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C155" t="inlineStr"/>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -2463,7 +3079,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C156" t="inlineStr"/>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -2476,7 +3096,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C157" t="inlineStr"/>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -2489,7 +3113,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C158" t="inlineStr"/>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -2502,7 +3130,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C159" t="inlineStr"/>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -2515,7 +3147,11 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C160" t="inlineStr"/>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>not found</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">

</xml_diff>

<commit_message>
added chrome restart + session handling
</commit_message>
<xml_diff>
--- a/zipcodes/CanadianPostalCodes202403_Processed.xlsx
+++ b/zipcodes/CanadianPostalCodes202403_Processed.xlsx
@@ -461,11 +461,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -478,11 +474,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -495,11 +487,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -512,11 +500,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -529,11 +513,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -546,11 +526,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -563,11 +539,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -580,11 +552,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -597,11 +565,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -614,11 +578,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -631,11 +591,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -648,11 +604,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -665,11 +617,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -682,11 +630,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -699,11 +643,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -716,11 +656,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -733,11 +669,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -750,11 +682,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -767,11 +695,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -784,11 +708,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -801,11 +721,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -818,11 +734,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -835,11 +747,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -852,11 +760,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -869,11 +773,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -886,11 +786,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -903,11 +799,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -920,11 +812,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -937,11 +825,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -954,11 +838,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -971,11 +851,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -988,11 +864,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1005,11 +877,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1022,11 +890,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1039,11 +903,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1056,11 +916,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1073,11 +929,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1090,11 +942,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1107,11 +955,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1124,11 +968,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1141,11 +981,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1158,11 +994,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1175,11 +1007,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1192,11 +1020,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1209,11 +1033,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1226,11 +1046,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1243,11 +1059,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1260,11 +1072,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1277,11 +1085,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1294,11 +1098,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1311,11 +1111,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1328,11 +1124,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1345,11 +1137,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1362,11 +1150,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1379,11 +1163,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1396,11 +1176,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1413,11 +1189,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1430,11 +1202,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1447,11 +1215,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1464,11 +1228,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1481,11 +1241,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1498,11 +1254,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1515,11 +1267,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1532,11 +1280,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1549,11 +1293,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1566,11 +1306,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1583,11 +1319,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1600,11 +1332,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1617,11 +1345,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1634,11 +1358,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1651,11 +1371,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1668,11 +1384,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1685,11 +1397,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1702,11 +1410,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1719,11 +1423,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1736,11 +1436,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1753,11 +1449,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1770,11 +1462,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1787,11 +1475,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1804,11 +1488,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1821,11 +1501,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1838,11 +1514,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1855,11 +1527,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1872,11 +1540,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1889,11 +1553,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1906,11 +1566,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1923,11 +1579,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1940,11 +1592,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1957,11 +1605,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1974,11 +1618,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1991,11 +1631,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2008,11 +1644,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2025,11 +1657,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2042,11 +1670,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2059,11 +1683,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2076,11 +1696,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2093,11 +1709,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2110,11 +1722,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2127,11 +1735,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2144,11 +1748,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2161,11 +1761,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2178,11 +1774,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2195,11 +1787,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2212,11 +1800,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2229,11 +1813,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2246,11 +1826,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2263,11 +1839,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2280,11 +1852,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2297,11 +1865,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2314,11 +1878,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2331,11 +1891,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2348,11 +1904,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2365,11 +1917,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2382,11 +1930,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2399,11 +1943,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2416,11 +1956,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2433,11 +1969,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2450,11 +1982,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2467,11 +1995,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2484,11 +2008,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2501,11 +2021,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2518,11 +2034,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2535,11 +2047,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2552,11 +2060,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2569,11 +2073,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2586,11 +2086,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2603,11 +2099,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2620,11 +2112,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2637,11 +2125,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2654,11 +2138,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2671,11 +2151,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2688,11 +2164,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2705,11 +2177,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2722,11 +2190,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2739,11 +2203,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2756,11 +2216,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2773,11 +2229,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2790,11 +2242,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2807,11 +2255,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2824,11 +2268,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2841,11 +2281,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2858,11 +2294,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2875,11 +2307,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2892,11 +2320,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2909,11 +2333,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2926,11 +2346,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2943,11 +2359,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2960,11 +2372,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2977,11 +2385,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
+      <c r="C150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2994,11 +2398,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3011,11 +2411,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3028,11 +2424,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3045,11 +2437,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3062,11 +2450,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3079,11 +2463,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3096,11 +2476,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3113,11 +2489,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3130,11 +2502,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3147,11 +2515,7 @@
           <t>AB</t>
         </is>
       </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>not found</t>
-        </is>
-      </c>
+      <c r="C160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">

</xml_diff>